<commit_message>
Introducing C for noGIL multithreading
Dramatically increased speed of program by implementing OpenAI API in C allowing multithreading with noGIL.
</commit_message>
<xml_diff>
--- a/Dependencies/Variables.xlsx
+++ b/Dependencies/Variables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\PycharmProjects\ChatGPT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\PycharmProjects\LLM_SchoolChoice\Dependencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57016BD7-F62B-45A2-A1AA-9C4CB8C25DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED38EAEC-D8C6-4462-A404-65DDA8CB7DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{54497F5C-4506-450A-8BAB-DF9BCB4BD4FB}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>kid</t>
   </si>
   <si>
-    <t>K level</t>
-  </si>
-  <si>
     <t>Both parents have a PhD.</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>in Bernal Heights</t>
+  </si>
+  <si>
+    <t>elementary school</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -578,7 +578,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -587,196 +587,196 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>